<commit_message>
remove unsupported function IFERROR() from mortgage_refinancing.xlsx
</commit_message>
<xml_diff>
--- a/kkapp/src/main/webapp/WEB-INF/books/mortgage_refinancing.xlsx
+++ b/kkapp/src/main/webapp/WEB-INF/books/mortgage_refinancing.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerry\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/keikai-oss/kkapp/src/main/webapp/WEB-INF/books/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F575DB-751E-6A4F-B1EF-9884FB10B281}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="20115" windowHeight="6480"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26120" windowHeight="17080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -142,24 +143,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="166" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="177" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -168,7 +169,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -180,7 +181,7 @@
     <font>
       <sz val="28"/>
       <color theme="2"/>
-      <name val="Cambria"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -188,21 +189,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1" tint="0.34998626667073579"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.34998626667073579"/>
-      <name val="Cambria"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.14999847407452621"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -357,8 +358,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment vertical="center"/>
@@ -411,10 +412,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="176" fontId="12" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="12" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -423,10 +424,10 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="176" fontId="13" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="12" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -463,48 +464,48 @@
     <xf numFmtId="9" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Date" xfId="2"/>
-    <cellStyle name="Fixed" xfId="3"/>
-    <cellStyle name="Heading 1 2" xfId="5"/>
-    <cellStyle name="Heading 2 2" xfId="6"/>
-    <cellStyle name="Heading 3 2" xfId="7"/>
-    <cellStyle name="Heading 4 2" xfId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Text" xfId="4"/>
+    <cellStyle name="Date" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Fixed" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Heading 1 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Heading 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Heading 3 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Heading 4 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Text" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -526,7 +527,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -601,6 +602,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -636,6 +654,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -811,26 +846,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" customWidth="1"/>
-    <col min="2" max="2" width="55.140625" customWidth="1"/>
-    <col min="3" max="4" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="1.796875" customWidth="1"/>
+    <col min="2" max="2" width="55.19921875" customWidth="1"/>
+    <col min="3" max="4" width="21.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="25.5" customHeight="1">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
     </row>
     <row r="2" spans="2:4" ht="12.75" customHeight="1">
       <c r="B2" s="2"/>
@@ -838,160 +873,160 @@
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="2:4" ht="18" customHeight="1">
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
     </row>
     <row r="4" spans="2:4" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="30"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="22">
         <v>0.06</v>
       </c>
     </row>
     <row r="5" spans="2:4" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="31"/>
+      <c r="C5" s="32"/>
       <c r="D5" s="23">
         <v>60</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="18" customHeight="1">
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
     </row>
     <row r="7" spans="2:4" ht="18" customHeight="1">
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="30"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="24">
         <v>180000</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="18" customHeight="1">
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="31"/>
+      <c r="C8" s="32"/>
       <c r="D8" s="25">
         <v>0.04</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="18" customHeight="1">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="31"/>
+      <c r="C9" s="32"/>
       <c r="D9" s="26">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="18" customHeight="1">
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="32"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="24">
         <v>210</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="18" customHeight="1">
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="33"/>
+      <c r="C11" s="36"/>
       <c r="D11" s="27">
         <v>0.03</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="18" customHeight="1">
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="31"/>
+      <c r="C12" s="32"/>
       <c r="D12" s="23">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="18" customHeight="1">
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="31"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="23">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="18" customHeight="1">
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
     </row>
     <row r="15" spans="2:4" ht="18" customHeight="1">
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="35"/>
+      <c r="C15" s="29"/>
       <c r="D15" s="20">
         <v>200</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="18" customHeight="1">
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="36"/>
+      <c r="C16" s="30"/>
       <c r="D16" s="21">
         <v>2000</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="18" customHeight="1">
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="34"/>
+      <c r="C17" s="28"/>
       <c r="D17" s="21">
         <v>200</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="18" customHeight="1">
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="35"/>
+      <c r="C18" s="29"/>
       <c r="D18" s="21">
         <v>100</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="18" customHeight="1">
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="36"/>
+      <c r="C19" s="30"/>
       <c r="D19" s="8">
-        <f>IFERROR(IF(SUM(D23),ROUND(D13/100*D23,0),""),"")</f>
+        <f>IF(SUM(D23),ROUND(D13/100*D23,0),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="18" customHeight="1">
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="37"/>
+      <c r="C20" s="31"/>
       <c r="D20" s="19">
-        <f>IFERROR(IF(SUM(D15:D19),SUM(D15:D19),""),"")</f>
+        <f>IF(SUM(D15:D19),SUM(D15:D19),"")</f>
         <v>2500</v>
       </c>
     </row>
@@ -1016,11 +1051,11 @@
         <v>21</v>
       </c>
       <c r="C23" s="18">
-        <f>IFERROR(IF(D9,PV(D8/12,D9*12-D10,-C24),""),"")</f>
+        <f>IF(D9,PV(D8/12,D9*12-D10,-C24),"")</f>
         <v>101308.00154925138</v>
       </c>
       <c r="D23" s="18">
-        <f>IFERROR(C23,"")</f>
+        <f>C23</f>
         <v>101308.00154925138</v>
       </c>
     </row>
@@ -1029,11 +1064,11 @@
         <v>22</v>
       </c>
       <c r="C24" s="14">
-        <f>IFERROR(IF(D8,PMT(D8/12,D9*12,-D7),""),"")</f>
+        <f>IF(D8,PMT(D8/12,D9*12,-D7),"")</f>
         <v>859.34753183782709</v>
       </c>
       <c r="D24" s="14">
-        <f>IFERROR(IF(D11,PMT(D11/12,D12*12,-D23),""),"")</f>
+        <f>IF(D11,PMT(D11/12,D12*12,-D23),"")</f>
         <v>699.61445883167187</v>
       </c>
     </row>
@@ -1043,7 +1078,7 @@
       </c>
       <c r="C25" s="16"/>
       <c r="D25" s="8">
-        <f>IFERROR(IF(SUM(C24)-SUM(D24),D20/(C24-D24),""),"")</f>
+        <f>IF(SUM(C24)-SUM(D24),D20/(C24-D24),"")</f>
         <v>15.651110649474978</v>
       </c>
     </row>
@@ -1052,11 +1087,11 @@
         <v>24</v>
       </c>
       <c r="C26" s="14">
-        <f>IFERROR(IF(D9,PV(D8/12,D9*12-D5-D10,-C24),""),"")</f>
+        <f>IF(D9,PV(D8/12,D9*12-D5-D10,-C24),"")</f>
         <v>66722.861566100299</v>
       </c>
       <c r="D26" s="14">
-        <f>IFERROR(IF(D11,PV(D11/12,D12*12-D5,-D24),""),"")</f>
+        <f>IF(D11,PV(D11/12,D12*12-D5,-D24),"")</f>
         <v>72453.299839073123</v>
       </c>
     </row>
@@ -1065,11 +1100,11 @@
         <v>25</v>
       </c>
       <c r="C27" s="13">
-        <f>IFERROR(IF(SUM(C26),C23-C26,""),"")</f>
+        <f>IF(SUM(C26),C23-C26,"")</f>
         <v>34585.139983151079</v>
       </c>
       <c r="D27" s="13">
-        <f>IFERROR(IF(SUM(D26),D23-D26,""),"")</f>
+        <f>IF(SUM(D26),D23-D26,"")</f>
         <v>28854.701710178255</v>
       </c>
     </row>
@@ -1078,11 +1113,11 @@
         <v>26</v>
       </c>
       <c r="C28" s="14">
-        <f>IFERROR(IF(SUM(C26),C24*D5,""),"")</f>
+        <f>IF(SUM(C26),C24*D5,"")</f>
         <v>51560.851910269623</v>
       </c>
       <c r="D28" s="14">
-        <f>IFERROR(IF(SUM(D26),D24*D5,""),"")</f>
+        <f>IF(SUM(D26),D24*D5,"")</f>
         <v>41976.867529900315</v>
       </c>
     </row>
@@ -1091,11 +1126,11 @@
         <v>27</v>
       </c>
       <c r="C29" s="13">
-        <f>IFERROR(IF(SUM(C26),C28-C27,""),"")</f>
+        <f>IF(SUM(C26),C28-C27,"")</f>
         <v>16975.711927118544</v>
       </c>
       <c r="D29" s="13">
-        <f>IFERROR(IF(SUM(D26),D28-D27,""),"")</f>
+        <f>IF(SUM(D26),D28-D27,"")</f>
         <v>13122.16581972206</v>
       </c>
     </row>
@@ -1104,11 +1139,11 @@
         <v>28</v>
       </c>
       <c r="C30" s="14">
-        <f>IFERROR(IF(SUM(C26),C29*D4,""),"")</f>
+        <f>IF(SUM(C26),C29*D4,"")</f>
         <v>1018.5427156271126</v>
       </c>
       <c r="D30" s="13">
-        <f>IFERROR(IF(SUM(D26),D29*D4,""),"")</f>
+        <f>IF(SUM(D26),D29*D4,"")</f>
         <v>787.32994918332361</v>
       </c>
     </row>
@@ -1117,11 +1152,11 @@
         <v>29</v>
       </c>
       <c r="C31" s="13">
-        <f>IFERROR(IF(SUM(C26),C29-C30,""),"")</f>
+        <f>IF(SUM(C26),C29-C30,"")</f>
         <v>15957.169211491431</v>
       </c>
       <c r="D31" s="18">
-        <f>IFERROR(IF(SUM(D26),D29-D30,""),"")</f>
+        <f>IF(SUM(D26),D29-D30,"")</f>
         <v>12334.835870538736</v>
       </c>
     </row>
@@ -1131,7 +1166,7 @@
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="14">
-        <f>IFERROR(IF(SUM(C31),C31-D31,""),"")</f>
+        <f>IF(SUM(C31),C31-D31,"")</f>
         <v>3622.3333409526949</v>
       </c>
     </row>
@@ -1141,7 +1176,7 @@
       </c>
       <c r="C33" s="16"/>
       <c r="D33" s="17">
-        <f>IFERROR(IF(SUM(C26),D32-D20,""),"")</f>
+        <f>IF(SUM(C26),D32-D20,"")</f>
         <v>1122.3333409526949</v>
       </c>
     </row>
@@ -1152,6 +1187,16 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
@@ -1161,16 +1206,6 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:D6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>